<commit_message>
Negative Test Cases for Product Module
</commit_message>
<xml_diff>
--- a/tests/artifact/data/Product.data.xlsx
+++ b/tests/artifact/data/Product.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>schema.path</t>
   </si>
@@ -106,7 +106,13 @@
     <t>valid.productcode</t>
   </si>
   <si>
-    <t>350</t>
+    <t>253</t>
+  </si>
+  <si>
+    <t>invalid.productcode</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1217,7 @@
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="1"/>
@@ -1324,8 +1330,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A14" s="5"/>
+    <row r="14" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" ht="23.1" customHeight="1" spans="1:1">
       <c r="A15" s="5"/>

</xml_diff>

<commit_message>
Product Module Negative Tests Updated
</commit_message>
<xml_diff>
--- a/tests/artifact/data/Product.data.xlsx
+++ b/tests/artifact/data/Product.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>schema.path</t>
   </si>
@@ -106,7 +106,40 @@
     <t>valid.productcode</t>
   </si>
   <si>
-    <t>350</t>
+    <t>253</t>
+  </si>
+  <si>
+    <t>invalid.productcode</t>
+  </si>
+  <si>
+    <t>test,asd2314, ,00,@#$123,$#@asd,1234</t>
+  </si>
+  <si>
+    <t>invalid.flag</t>
+  </si>
+  <si>
+    <t>123,aw234,@#!w34,test, ,012@!#,-2098</t>
+  </si>
+  <si>
+    <t>invalid.integervalue</t>
+  </si>
+  <si>
+    <t>@-123,aw234,@#!w34,test, ,012@!#,-(*2098</t>
+  </si>
+  <si>
+    <t>invalid.uomid</t>
+  </si>
+  <si>
+    <t>invalid.godownflag</t>
+  </si>
+  <si>
+    <t>invalid.qty</t>
+  </si>
+  <si>
+    <t>invalid.rate</t>
+  </si>
+  <si>
+    <t>invalid.categorycode</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1244,7 @@
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="1"/>
@@ -1324,29 +1357,69 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A15" s="5"/>
-    </row>
-    <row r="16" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A16" s="5"/>
-    </row>
-    <row r="17" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A17" s="5"/>
-    </row>
-    <row r="18" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A18" s="5"/>
-    </row>
-    <row r="19" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A19" s="5"/>
-    </row>
-    <row r="20" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A20" s="5"/>
-    </row>
-    <row r="21" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A21" s="5"/>
+    <row r="14" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" ht="23.1" customHeight="1" spans="1:1">
       <c r="A22" s="5"/>

</xml_diff>